<commit_message>
stator and outer frame done
</commit_message>
<xml_diff>
--- a/raw_blade_data/blade_info.xlsx
+++ b/raw_blade_data/blade_info.xlsx
@@ -16,15 +16,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
   <si>
-    <t>blade count</t>
+    <t>rotor blade count</t>
   </si>
   <si>
     <t>level</t>
   </si>
   <si>
     <t>count</t>
+  </si>
+  <si>
+    <t>stator blade count</t>
   </si>
 </sst>
 </file>
@@ -35,17 +38,10 @@
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="0.000_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="0.000_ "/>
   </numFmts>
-  <fonts count="21">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -503,48 +499,51 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -554,109 +553,109 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1006,15 +1005,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="B2:I22"/>
+  <dimension ref="B2:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="14.1111111111111" customWidth="1"/>
+    <col min="2" max="2" width="20.0833333333333" customWidth="1"/>
     <col min="4" max="4" width="15.5555555555556" customWidth="1"/>
     <col min="5" max="5" width="15.2222222222222"/>
   </cols>
@@ -1267,24 +1266,226 @@
       <c r="C17" s="1"/>
     </row>
     <row r="18" spans="2:3">
-      <c r="B18" s="1"/>
+      <c r="B18" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="C18" s="1"/>
     </row>
     <row r="19" spans="2:3">
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-    </row>
-    <row r="20" spans="2:3">
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-    </row>
-    <row r="21" spans="2:3">
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-    </row>
-    <row r="22" spans="2:3">
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
+      <c r="B19" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5">
+      <c r="B20" s="1">
+        <v>1</v>
+      </c>
+      <c r="C20" s="1">
+        <v>42</v>
+      </c>
+      <c r="D20">
+        <f>$D$2/C20</f>
+        <v>8.57142857142857</v>
+      </c>
+      <c r="E20">
+        <f>D20/2</f>
+        <v>4.28571428571429</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5">
+      <c r="B21" s="1">
+        <v>2</v>
+      </c>
+      <c r="C21" s="1">
+        <v>44</v>
+      </c>
+      <c r="D21">
+        <f t="shared" ref="D21:D32" si="2">$D$2/C21</f>
+        <v>8.18181818181818</v>
+      </c>
+      <c r="E21">
+        <f t="shared" ref="E21:E32" si="3">D21/2</f>
+        <v>4.09090909090909</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5">
+      <c r="B22" s="1">
+        <v>3</v>
+      </c>
+      <c r="C22" s="1">
+        <v>46</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="2"/>
+        <v>7.82608695652174</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="3"/>
+        <v>3.91304347826087</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5">
+      <c r="B23" s="1">
+        <v>4</v>
+      </c>
+      <c r="C23" s="1">
+        <v>48</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="2"/>
+        <v>7.5</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="3"/>
+        <v>3.75</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5">
+      <c r="B24" s="1">
+        <v>5</v>
+      </c>
+      <c r="C24" s="1">
+        <v>50</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="2"/>
+        <v>7.2</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="3"/>
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5">
+      <c r="B25" s="1">
+        <v>6</v>
+      </c>
+      <c r="C25" s="1">
+        <v>52</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="2"/>
+        <v>6.92307692307692</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="3"/>
+        <v>3.46153846153846</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5">
+      <c r="B26" s="1">
+        <v>7</v>
+      </c>
+      <c r="C26" s="1">
+        <v>54</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="2"/>
+        <v>6.66666666666667</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="3"/>
+        <v>3.33333333333333</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5">
+      <c r="B27" s="1">
+        <v>8</v>
+      </c>
+      <c r="C27" s="1">
+        <v>56</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="2"/>
+        <v>6.42857142857143</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="3"/>
+        <v>3.21428571428571</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5">
+      <c r="B28" s="1">
+        <v>9</v>
+      </c>
+      <c r="C28" s="1">
+        <v>58</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="2"/>
+        <v>6.20689655172414</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="3"/>
+        <v>3.10344827586207</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5">
+      <c r="B29" s="1">
+        <v>10</v>
+      </c>
+      <c r="C29" s="1">
+        <v>60</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5">
+      <c r="B30" s="1">
+        <v>11</v>
+      </c>
+      <c r="C30" s="1">
+        <v>62</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="2"/>
+        <v>5.80645161290323</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="3"/>
+        <v>2.90322580645161</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5">
+      <c r="B31" s="1">
+        <v>12</v>
+      </c>
+      <c r="C31" s="1">
+        <v>64</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="2"/>
+        <v>5.625</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="3"/>
+        <v>2.8125</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5">
+      <c r="B32" s="1">
+        <v>13</v>
+      </c>
+      <c r="C32" s="1">
+        <v>66</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="2"/>
+        <v>5.45454545454545</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="3"/>
+        <v>2.72727272727273</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>